<commit_message>
changes made on main/test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelRequests.xlsx
+++ b/src/test/resources/TestData/ExcelRequests.xlsx
@@ -7,7 +7,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="postRequest " sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
     <t>8icf</t>
   </si>
   <si>
-    <t xml:space="preserve"> /deleteuser/10680</t>
+    <t xml:space="preserve"> /deleteuser/10970</t>
   </si>
   <si>
     <t xml:space="preserve"> /deleteuser/</t>
@@ -625,7 +625,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:K25"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1521,8 +1521,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1600,7 +1600,7 @@
         <v>57</v>
       </c>
       <c r="B9">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10">
@@ -2360,7 +2360,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>